<commit_message>
changed excel sheets to correct one
</commit_message>
<xml_diff>
--- a/CSBA_Excel/StatData.xlsx
+++ b/CSBA_Excel/StatData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCD8D5B-7E51-430D-90BF-6F00B6958108}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696BBBC7-BF62-41B2-84FE-CAC91264A958}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5775" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Season" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="711">
   <si>
     <t>T</t>
   </si>
@@ -2038,12 +2038,6 @@
     <t>HIT_BY_PITCH</t>
   </si>
   <si>
-    <t>BASE_ON_BALLS</t>
-  </si>
-  <si>
-    <t>STRIKE_OUT</t>
-  </si>
-  <si>
     <t>TRIPLE</t>
   </si>
   <si>
@@ -2122,9 +2116,6 @@
     <t>EARNED_RUN</t>
   </si>
   <si>
-    <t>STRIKEOUT</t>
-  </si>
-  <si>
     <t>HOMERUNS_ALLOWED</t>
   </si>
   <si>
@@ -2147,6 +2138,18 @@
   </si>
   <si>
     <t>VARCHAR(5)</t>
+  </si>
+  <si>
+    <t>BASE_ON_BALLS_PITCHERS</t>
+  </si>
+  <si>
+    <t>STRIKEOUT_PITCHER</t>
+  </si>
+  <si>
+    <t>BASE_ON_BALLS_BATTERS</t>
+  </si>
+  <si>
+    <t>STRIKEOUT_BATTERS</t>
   </si>
 </sst>
 </file>
@@ -2560,7 +2563,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,8 +2604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2625,8 +2628,8 @@
     <col min="16" max="16" width="18.85546875" style="6" customWidth="1"/>
     <col min="17" max="17" width="16.140625" style="6" customWidth="1"/>
     <col min="18" max="18" width="14.28515625" style="6" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" style="6" customWidth="1"/>
-    <col min="20" max="20" width="14" style="6" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" style="6" customWidth="1"/>
+    <col min="20" max="20" width="20" style="6" customWidth="1"/>
     <col min="21" max="21" width="21.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.28515625" style="6" customWidth="1"/>
     <col min="23" max="28" width="9.140625" style="8"/>
@@ -2646,58 +2649,58 @@
         <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="F1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -2711,61 +2714,61 @@
         <v>36</v>
       </c>
       <c r="D2" t="s">
+        <v>686</v>
+      </c>
+      <c r="E2" t="s">
+        <v>685</v>
+      </c>
+      <c r="F2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>688</v>
       </c>
-      <c r="E2" t="s">
-        <v>687</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" s="6" t="s">
         <v>689</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>690</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>691</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>692</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="6" t="s">
+        <v>694</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>693</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>694</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="N2" s="6" t="s">
+        <v>695</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>695</v>
-      </c>
-      <c r="N2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>697</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="Q2" s="6" t="s">
+        <v>700</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>698</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="U2" s="6" t="s">
         <v>699</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>703</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>700</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>673</v>
-      </c>
-      <c r="T2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>701</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>702</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -12496,8 +12499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12519,8 +12522,8 @@
     <col min="15" max="15" width="14.28515625" style="6" customWidth="1"/>
     <col min="16" max="16" width="19.5703125" style="6" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" style="6" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="6" customWidth="1"/>
+    <col min="18" max="18" width="24.85546875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="21.7109375" style="6" customWidth="1"/>
     <col min="20" max="20" width="14" style="6" customWidth="1"/>
     <col min="21" max="21" width="17.28515625" style="6" customWidth="1"/>
   </cols>
@@ -12539,55 +12542,55 @@
         <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="F1" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -12601,34 +12604,34 @@
         <v>36</v>
       </c>
       <c r="D2" t="s">
+        <v>678</v>
+      </c>
+      <c r="E2" t="s">
+        <v>679</v>
+      </c>
+      <c r="F2" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>677</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>676</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>680</v>
       </c>
-      <c r="E2" t="s">
-        <v>681</v>
-      </c>
-      <c r="F2" t="s">
-        <v>686</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>679</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>685</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>678</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>682</v>
-      </c>
       <c r="K2" s="6" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>669</v>
@@ -12643,16 +12646,16 @@
         <v>672</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>673</v>
+        <v>709</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>674</v>
+        <v>710</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>